<commit_message>
Mean diff, pairwise test fn, res check fn.
</commit_message>
<xml_diff>
--- a/eg_data/NHANES/PF/n1776/n1776_Div Grouping.xlsx
+++ b/eg_data/NHANES/PF/n1776/n1776_Div Grouping.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sadoh\OneDrive\Documents\GitHub\DietR\eg_data\NHANES\PF\n1777\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sadoh\OneDrive\Documents\GitHub\DietR\eg_data\NHANES\PF\n1776\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44991EBF-CCCA-4191-9580-390163E607CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{325A2066-6CE2-48FC-9BD6-AA019F59FB3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32295" yWindow="-2610" windowWidth="16155" windowHeight="14475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33450" yWindow="-3075" windowWidth="14220" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
   <si>
     <t>DivNA</t>
   </si>
@@ -90,13 +90,34 @@
   </si>
   <si>
     <t>1777 rows remained.</t>
+  </si>
+  <si>
+    <t>Remove one outlier in HDL</t>
+  </si>
+  <si>
+    <t>1776 rows remained.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          F   M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  DivNA 467 419</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Div0  311 252</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Div1   88  81</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Div2   82  76</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,6 +143,12 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -159,7 +186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -176,6 +203,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,12 +497,12 @@
     <col min="5" max="6" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="s">
         <v>0</v>
@@ -489,7 +517,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
@@ -506,7 +534,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>5</v>
       </c>
@@ -523,7 +551,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
@@ -540,65 +568,110 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="1"/>
-      <c r="C13" s="2" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+      <c r="C17" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="3" t="s">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C18" s="4">
         <v>886</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D18" s="4">
         <v>563</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E18" s="4">
         <v>169</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F18" s="4">
         <v>158</v>
       </c>
-      <c r="G14">
-        <f>SUM(C14:F14)</f>
+      <c r="G18">
+        <f>SUM(C18:F18)</f>
         <v>1776</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="6" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>